<commit_message>
Se agrego boton para agregar filas manualmente
</commit_message>
<xml_diff>
--- a/APP WEB/Facturas.xlsx
+++ b/APP WEB/Facturas.xlsx
@@ -460,7 +460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -629,6 +629,258 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SKM_C335124092312180_0026.jpg</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>12/07/2024</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>200,00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>165,29</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>21,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SKM_C335124092312180_0033.jpg</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>18/07/2024</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>11307</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>170,01</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>140,50</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SKM_C335124092312180_0032.jpg</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>28/08/2024</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>13536</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>150,00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>123,97</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>21,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SKM_C335124092312180_0032.jpg</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>28/08/2024</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3.536</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>150,00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>123,97</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>21,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SKM_C335124092312180_0030.jpg</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>16/08/2024</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>12980</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>200,00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>165,29</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>21,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SKM_C335124092312180_0031.jpg</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>21/08/2024</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>6938R</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>150,00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>123,97</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>21,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SKM_C335124092312180_0028.jpg</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>29/07/2024</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>9838R</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>47,06</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>38,89</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>8,17</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>01/01/2024</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>9218</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>100,21</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>12,2</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>